<commit_message>
change last time to 1995 - hyang
</commit_message>
<xml_diff>
--- a/topo_alarm/alarm.xlsx
+++ b/topo_alarm/alarm.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/22205/Desktop/analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/22205/workspace/TopoViewer/topo_alarm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AAFE6BA-7815-924C-A070-87D832CC13C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D31A5A-19C6-4645-BF9E-EED605A0B33F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2707,7 +2707,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="298">
   <si>
     <t>Acked</t>
   </si>
@@ -3663,6 +3663,30 @@
   </si>
   <si>
     <t>2019-04-19 12:54:46</t>
+  </si>
+  <si>
+    <t>1995-09-19 12:54:56</t>
+  </si>
+  <si>
+    <t>1995-09-19 12:48:56</t>
+  </si>
+  <si>
+    <t>1995-09-19 12:48:55</t>
+  </si>
+  <si>
+    <t>1995-09-19 12:48:52</t>
+  </si>
+  <si>
+    <t>1995-09-19 12:54:36</t>
+  </si>
+  <si>
+    <t>1995-09-19 12:54:13</t>
+  </si>
+  <si>
+    <t>1995-09-19 12:54:11</t>
+  </si>
+  <si>
+    <t>1995-09-19 12:54:46</t>
   </si>
 </sst>
 </file>
@@ -4060,8 +4084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:GK12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BD1" workbookViewId="0">
-      <selection activeCell="BY13" sqref="BY13"/>
+    <sheetView tabSelected="1" topLeftCell="BM1" workbookViewId="0">
+      <selection activeCell="BZ11" sqref="BZ11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4854,7 +4878,7 @@
         <v>282</v>
       </c>
       <c r="BZ2" s="3" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="CC2" t="s">
         <v>191</v>
@@ -4980,7 +5004,7 @@
         <v>282</v>
       </c>
       <c r="BZ3" s="3" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="CC3" t="s">
         <v>191</v>
@@ -5103,7 +5127,7 @@
         <v>283</v>
       </c>
       <c r="BZ4" s="3" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="CC4" t="s">
         <v>191</v>
@@ -5226,7 +5250,7 @@
         <v>284</v>
       </c>
       <c r="BZ5" s="3" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="CC5" t="s">
         <v>191</v>
@@ -5349,7 +5373,7 @@
         <v>285</v>
       </c>
       <c r="BZ6" s="3" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="CC6" t="s">
         <v>191</v>
@@ -5472,7 +5496,7 @@
         <v>285</v>
       </c>
       <c r="BZ7" s="3" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="CC7" t="s">
         <v>191</v>
@@ -5597,7 +5621,7 @@
         <v>286</v>
       </c>
       <c r="BZ8" s="3" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="CC8" t="s">
         <v>191</v>
@@ -5722,7 +5746,7 @@
         <v>287</v>
       </c>
       <c r="BZ9" s="3" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="CC9" t="s">
         <v>191</v>
@@ -5848,7 +5872,7 @@
         <v>288</v>
       </c>
       <c r="BZ10" s="3" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="CC10" t="s">
         <v>191</v>
@@ -5973,7 +5997,7 @@
         <v>289</v>
       </c>
       <c r="BZ11" s="3" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="CC11" t="s">
         <v>191</v>

</xml_diff>

<commit_message>
update fake data - hyang
</commit_message>
<xml_diff>
--- a/topo_alarm/alarm.xlsx
+++ b/topo_alarm/alarm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/22205/Desktop/topo_alarm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92B1D9D-2987-B24E-9DB6-6E6B785075A8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61ACFF4-9EEE-374C-A5D6-5226AEAD9B04}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2711,7 +2711,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="323">
   <si>
     <t>Acked</t>
   </si>
@@ -3759,6 +3759,12 @@
   </si>
   <si>
     <t>2019-04-20 12:54:46</t>
+  </si>
+  <si>
+    <t>FJDSIGOI</t>
+  </si>
+  <si>
+    <t>YUOYIUGTF</t>
   </si>
 </sst>
 </file>
@@ -4178,10 +4184,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:GK23"/>
+  <dimension ref="A1:GK25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BF1" workbookViewId="0">
-      <selection activeCell="BO23" sqref="BO23"/>
+    <sheetView tabSelected="1" topLeftCell="CP1" workbookViewId="0">
+      <selection activeCell="CV25" sqref="CV25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7680,6 +7686,242 @@
         <v>274</v>
       </c>
     </row>
+    <row r="24" spans="1:186" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B24" t="s">
+        <v>191</v>
+      </c>
+      <c r="C24" t="s">
+        <v>191</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E24">
+        <v>9498558833</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="W24" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="AO24" t="s">
+        <v>191</v>
+      </c>
+      <c r="AP24" t="s">
+        <v>191</v>
+      </c>
+      <c r="AQ24" t="s">
+        <v>191</v>
+      </c>
+      <c r="AR24" t="s">
+        <v>191</v>
+      </c>
+      <c r="AS24" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="BC24" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="BD24" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="BO24" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="BZ24" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="CC24" t="s">
+        <v>191</v>
+      </c>
+      <c r="CD24" t="s">
+        <v>191</v>
+      </c>
+      <c r="CJ24" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="CV24" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="CW24" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="DN24" t="s">
+        <v>196</v>
+      </c>
+      <c r="DO24" s="2"/>
+      <c r="DQ24" s="2"/>
+      <c r="DR24" t="s">
+        <v>191</v>
+      </c>
+      <c r="DS24" t="s">
+        <v>191</v>
+      </c>
+      <c r="DW24" t="s">
+        <v>191</v>
+      </c>
+      <c r="DX24" t="s">
+        <v>191</v>
+      </c>
+      <c r="DY24" t="s">
+        <v>191</v>
+      </c>
+      <c r="DZ24" t="s">
+        <v>191</v>
+      </c>
+      <c r="EA24" t="s">
+        <v>191</v>
+      </c>
+      <c r="EB24" t="s">
+        <v>191</v>
+      </c>
+      <c r="EC24" t="s">
+        <v>191</v>
+      </c>
+      <c r="ED24" t="s">
+        <v>191</v>
+      </c>
+      <c r="EE24" t="s">
+        <v>191</v>
+      </c>
+      <c r="EF24" t="s">
+        <v>191</v>
+      </c>
+      <c r="GD24" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="25" spans="1:186" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B25" t="s">
+        <v>191</v>
+      </c>
+      <c r="C25" t="s">
+        <v>191</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E25">
+        <v>9498558833</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="W25" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="AO25" t="s">
+        <v>191</v>
+      </c>
+      <c r="AP25" t="s">
+        <v>191</v>
+      </c>
+      <c r="AQ25" t="s">
+        <v>191</v>
+      </c>
+      <c r="AR25" t="s">
+        <v>191</v>
+      </c>
+      <c r="AS25" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="BC25" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="BD25" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="BO25" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="BZ25" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="CC25" t="s">
+        <v>191</v>
+      </c>
+      <c r="CD25" t="s">
+        <v>191</v>
+      </c>
+      <c r="CJ25" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="CV25" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="CW25" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="DN25" t="s">
+        <v>196</v>
+      </c>
+      <c r="DO25" s="2"/>
+      <c r="DQ25" s="2"/>
+      <c r="DR25" t="s">
+        <v>191</v>
+      </c>
+      <c r="DS25" t="s">
+        <v>191</v>
+      </c>
+      <c r="DW25" t="s">
+        <v>191</v>
+      </c>
+      <c r="DX25" t="s">
+        <v>191</v>
+      </c>
+      <c r="DY25" t="s">
+        <v>191</v>
+      </c>
+      <c r="DZ25" t="s">
+        <v>191</v>
+      </c>
+      <c r="EA25" t="s">
+        <v>191</v>
+      </c>
+      <c r="EB25" t="s">
+        <v>191</v>
+      </c>
+      <c r="EC25" t="s">
+        <v>191</v>
+      </c>
+      <c r="ED25" t="s">
+        <v>191</v>
+      </c>
+      <c r="EE25" t="s">
+        <v>191</v>
+      </c>
+      <c r="EF25" t="s">
+        <v>191</v>
+      </c>
+      <c r="GD25" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>